<commit_message>
small updates july 2024
</commit_message>
<xml_diff>
--- a/research/Monte_carlo/output/sensitivity_results_for_report.xlsx
+++ b/research/Monte_carlo/output/sensitivity_results_for_report.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kwrwater-my.sharepoint.com/personal/alex_hockin_kwrwater_nl/Documents/VEWIN Permatie/pipepermcalc/research/Monte_carlo/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{281B2A1F-EACC-47C1-9449-F127ED4D3B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAB79E02-2ADD-4144-98EC-B754A0CC3F1A}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="8_{281B2A1F-EACC-47C1-9449-F127ED4D3B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E388454-E71F-4CB2-A20A-52746408AFE7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21140" xr2:uid="{2406CEAD-82FB-4CF0-ABAD-77E91FCE0AED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{2406CEAD-82FB-4CF0-ABAD-77E91FCE0AED}"/>
   </bookViews>
   <sheets>
     <sheet name="df_analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">df_analysis!$E$74:$H$74</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
   <si>
     <t>W</t>
   </si>
@@ -508,6 +509,12 @@
   </si>
   <si>
     <t>Difference gemiddeld – na stagnatie due to stagnation factor?</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>exposure</t>
   </si>
 </sst>
 </file>
@@ -806,7 +813,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -814,6 +820,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
@@ -1134,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2E1DA2-E553-489B-9336-8780D91A841A}">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
@@ -2692,10 +2699,10 @@
       <c r="G56" t="s">
         <v>12</v>
       </c>
-      <c r="H56" s="34" t="s">
+      <c r="H56" t="s">
         <v>52</v>
       </c>
-      <c r="I56" s="34" t="s">
+      <c r="I56" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2710,10 +2717,10 @@
       <c r="G57" s="3">
         <v>10.000008837419362</v>
       </c>
-      <c r="H57" s="35" t="s">
+      <c r="H57" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="I57" s="35" t="s">
+      <c r="I57" s="34" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2728,8 +2735,8 @@
       <c r="G58" s="3">
         <v>6.2081637757268862</v>
       </c>
-      <c r="H58" s="36"/>
-      <c r="I58" s="35" t="s">
+      <c r="H58" s="35"/>
+      <c r="I58" s="34" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2744,7 +2751,7 @@
       <c r="G59" s="3">
         <v>2.5470368419237261</v>
       </c>
-      <c r="I59" s="35" t="s">
+      <c r="I59" s="34" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2759,10 +2766,10 @@
       <c r="G60" s="3">
         <v>0</v>
       </c>
-      <c r="H60" s="35" t="s">
+      <c r="H60" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="I60" s="35"/>
+      <c r="I60" s="34"/>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D61" s="4"/>
@@ -2775,7 +2782,7 @@
       <c r="G61" s="3">
         <v>0</v>
       </c>
-      <c r="H61" s="36" t="s">
+      <c r="H61" s="35" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2790,7 +2797,7 @@
       <c r="G62" s="3">
         <v>0</v>
       </c>
-      <c r="I62" s="35"/>
+      <c r="I62" s="34"/>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D63" s="4"/>
@@ -2804,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="3"/>
-      <c r="I63" s="35"/>
+      <c r="I63" s="34"/>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D64" s="4"/>
@@ -2818,7 +2825,7 @@
         <v>-0.43354859965588843</v>
       </c>
       <c r="H64" s="3"/>
-      <c r="I64" s="35" t="s">
+      <c r="I64" s="34" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2834,7 +2841,7 @@
         <v>-0.62973021188383482</v>
       </c>
       <c r="H65" s="3"/>
-      <c r="I65" s="35"/>
+      <c r="I65" s="34"/>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D66" s="4"/>
@@ -2848,7 +2855,7 @@
         <v>-4.3422103927938389</v>
       </c>
       <c r="H66" s="3"/>
-      <c r="I66" s="35"/>
+      <c r="I66" s="34"/>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D67" s="4"/>
@@ -2889,10 +2896,9 @@
       <c r="G69" s="3">
         <v>-9.0909157305924797</v>
       </c>
-      <c r="H69" s="37" t="s">
+      <c r="H69" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="I69" s="34"/>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D70" s="4"/>
@@ -2905,13 +2911,11 @@
       <c r="G70" s="3">
         <v>-9.0909090909091468</v>
       </c>
-      <c r="I70" s="34"/>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D71" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I71" s="34"/>
     </row>
     <row r="72" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="73" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3136,4 +3140,112 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEBF52AA-0C01-447C-9C32-21FFC1CC032C}">
+  <dimension ref="C3:Q11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C4" s="37">
+        <v>0.33</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>D4*C4</f>
+        <v>0.66</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C5" s="37">
+        <f>1-C4</f>
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <f>D5*C5</f>
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>SUM(E4:E5)</f>
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f>33.3*2</f>
+        <v>66.599999999999994</v>
+      </c>
+      <c r="G10">
+        <f>3*2</f>
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <f>6*7</f>
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <f>SUM(G10:H10)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f>I10/10</f>
+        <v>4.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>